<commit_message>
addOrder improved -> amount cannot be negative anymore
</commit_message>
<xml_diff>
--- a/DONE.xlsx
+++ b/DONE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jonas\Programmierung\Ionic\WildShop\WNodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29D44C2-532E-40B2-8312-015034D3B80D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3F8349-F5EE-43E5-B247-093B8A8E94CD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8892" xr2:uid="{548DDF21-B18E-4EE1-82BD-5D6514E54740}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8892" xr2:uid="{548DDF21-B18E-4EE1-82BD-5D6514E54740}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Funktionalität</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Bestätigungsmail fehlt</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>noch nicht auf allen Seiten implementiert</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61DAD81-DA30-4CA7-A394-CE52C647E1CE}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,6 +474,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>